<commit_message>
Avalição GQA preenchida e finalizada
</commit_message>
<xml_diff>
--- a/Processo/Avaliação/GQA-Avaliação Processo.xlsx
+++ b/Processo/Avaliação/GQA-Avaliação Processo.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="39">
   <si>
     <t>INSTRUÇÕES</t>
   </si>
@@ -88,6 +88,20 @@
     </r>
   </si>
   <si>
+    <t>G5-GQA-PlanodeGarantiadaQualidade-Template.docx</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="13"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>X</t>
+    </r>
+  </si>
+  <si>
     <t>(T,L,P,N,NA)</t>
   </si>
   <si>
@@ -116,17 +130,6 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="15"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>X</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
         <b val="1"/>
         <sz val="10"/>
         <color indexed="8"/>
@@ -173,11 +176,17 @@
         <b val="1"/>
         <u val="single"/>
         <sz val="10"/>
-        <color indexed="15"/>
+        <color indexed="13"/>
         <rFont val="Arial"/>
       </rPr>
       <t>X</t>
     </r>
+  </si>
+  <si>
+    <t>Solicitacao_Acao_Corretiva.xlsx</t>
+  </si>
+  <si>
+    <t>ComunicaçãoSuperior.docx</t>
   </si>
   <si>
     <t>Atributos de Processo</t>
@@ -204,9 +213,6 @@
       </rPr>
       <t>As evidências apresentadas para este resultado permitem assegurar: (i) que foi definida uma política organizacional estabelecendo as expectativas da organização para a execução do processo e que esta política é conhecida e de fácil acesso aos interessados? (ii) que a política organizacional foi atualizada, quando necessário? (iii) que a política organizacional tem respaldo da alta administração (por exemplo, por meio de aprovação da alta administração)?</t>
     </r>
-  </si>
-  <si>
-    <t>G5-GQA-PlanodeGarantiadaQualidade-Template.docx</t>
   </si>
   <si>
     <r>
@@ -269,7 +275,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <color indexed="13"/>
+        <color indexed="14"/>
         <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve"> 
@@ -406,21 +412,21 @@
       <name val="Arial"/>
     </font>
     <font>
+      <u val="single"/>
       <sz val="10"/>
       <color indexed="13"/>
       <name val="Arial"/>
     </font>
     <font>
-      <u val="single"/>
       <sz val="10"/>
-      <color indexed="15"/>
+      <color indexed="14"/>
       <name val="Arial"/>
     </font>
     <font>
       <b val="1"/>
       <u val="single"/>
       <sz val="10"/>
-      <color indexed="15"/>
+      <color indexed="13"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -437,12 +443,12 @@
     </font>
     <font>
       <sz val="10"/>
-      <color indexed="13"/>
+      <color indexed="14"/>
       <name val="Times New Roman"/>
     </font>
     <font>
       <sz val="12"/>
-      <color indexed="13"/>
+      <color indexed="14"/>
       <name val="Times New Roman"/>
     </font>
     <font>
@@ -478,7 +484,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="14"/>
+        <fgColor indexed="15"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -1003,33 +1009,36 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="26" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="26" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1077,9 +1086,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="6" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
@@ -1111,9 +1117,9 @@
       <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ffc0c0c0"/>
       <rgbColor rgb="ffccffcc"/>
+      <rgbColor rgb="ff0000ff"/>
       <rgbColor rgb="ff0000d4"/>
       <rgbColor rgb="fffcf305"/>
-      <rgbColor rgb="ff0000ff"/>
       <rgbColor rgb="ffffff99"/>
       <rgbColor rgb="ffdd0806"/>
     </indexedColors>
@@ -2423,52 +2429,56 @@
       <c r="E5" s="30"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="37"/>
+      <c r="A6" t="s" s="37">
+        <v>19</v>
+      </c>
       <c r="B6" s="38"/>
-      <c r="C6" s="38"/>
+      <c r="C6" t="s" s="39">
+        <v>20</v>
+      </c>
       <c r="D6" s="38"/>
       <c r="E6" s="30"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="37"/>
+      <c r="A7" s="40"/>
       <c r="B7" s="38"/>
       <c r="C7" s="38"/>
       <c r="D7" s="38"/>
       <c r="E7" s="30"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="39"/>
+      <c r="A8" s="41"/>
       <c r="B8" s="38"/>
       <c r="C8" s="38"/>
       <c r="D8" s="38"/>
       <c r="E8" s="30"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="39"/>
+      <c r="A9" s="41"/>
       <c r="B9" s="38"/>
       <c r="C9" s="38"/>
       <c r="D9" s="38"/>
       <c r="E9" s="30"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="39"/>
+      <c r="A10" s="41"/>
       <c r="B10" s="38"/>
       <c r="C10" s="38"/>
       <c r="D10" s="38"/>
       <c r="E10" s="30"/>
     </row>
     <row r="11" ht="13.65" customHeight="1">
-      <c r="A11" s="40"/>
-      <c r="B11" t="s" s="41">
-        <v>19</v>
-      </c>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42"/>
+      <c r="A11" s="42"/>
+      <c r="B11" t="s" s="43">
+        <v>21</v>
+      </c>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
       <c r="E11" s="30"/>
     </row>
     <row r="12" ht="78.75" customHeight="1">
       <c r="A12" t="s" s="34">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B12" s="35"/>
       <c r="C12" s="36"/>
@@ -2476,12 +2486,12 @@
       <c r="E12" s="30"/>
     </row>
     <row r="13" ht="13.65" customHeight="1">
-      <c r="A13" t="s" s="43">
-        <v>21</v>
+      <c r="A13" t="s" s="37">
+        <v>23</v>
       </c>
       <c r="B13" s="38"/>
-      <c r="C13" t="s" s="44">
-        <v>22</v>
+      <c r="C13" t="s" s="39">
+        <v>20</v>
       </c>
       <c r="D13" s="38"/>
       <c r="E13" s="30"/>
@@ -2494,51 +2504,51 @@
       <c r="E14" s="30"/>
     </row>
     <row r="15" ht="13.65" customHeight="1">
-      <c r="A15" s="37"/>
+      <c r="A15" s="46"/>
       <c r="B15" s="38"/>
       <c r="C15" s="38"/>
       <c r="D15" s="38"/>
       <c r="E15" s="30"/>
     </row>
     <row r="16" ht="13.65" customHeight="1">
-      <c r="A16" s="37"/>
+      <c r="A16" s="46"/>
       <c r="B16" s="38"/>
       <c r="C16" s="38"/>
       <c r="D16" s="38"/>
       <c r="E16" s="30"/>
     </row>
     <row r="17" ht="13.65" customHeight="1">
-      <c r="A17" s="37"/>
+      <c r="A17" s="46"/>
       <c r="B17" s="38"/>
       <c r="C17" s="38"/>
       <c r="D17" s="38"/>
       <c r="E17" s="30"/>
     </row>
     <row r="18" ht="13.65" customHeight="1">
-      <c r="A18" s="40"/>
-      <c r="B18" t="s" s="41">
-        <v>19</v>
-      </c>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
+      <c r="A18" s="42"/>
+      <c r="B18" t="s" s="43">
+        <v>21</v>
+      </c>
+      <c r="C18" s="44"/>
+      <c r="D18" s="44"/>
       <c r="E18" s="30"/>
     </row>
     <row r="19" ht="35.65" customHeight="1">
       <c r="A19" t="s" s="34">
-        <v>23</v>
-      </c>
-      <c r="B19" s="46"/>
-      <c r="C19" s="46"/>
+        <v>24</v>
+      </c>
+      <c r="B19" s="47"/>
+      <c r="C19" s="47"/>
       <c r="D19" s="36"/>
       <c r="E19" s="30"/>
     </row>
     <row r="20" ht="13.65" customHeight="1">
-      <c r="A20" t="s" s="43">
-        <v>24</v>
-      </c>
-      <c r="B20" s="47"/>
-      <c r="C20" t="s" s="48">
-        <v>22</v>
+      <c r="A20" t="s" s="37">
+        <v>25</v>
+      </c>
+      <c r="B20" s="48"/>
+      <c r="C20" t="s" s="49">
+        <v>20</v>
       </c>
       <c r="D20" s="38"/>
       <c r="E20" s="30"/>
@@ -2551,193 +2561,201 @@
       <c r="E21" s="30"/>
     </row>
     <row r="22" ht="13.65" customHeight="1">
-      <c r="A22" s="37"/>
+      <c r="A22" s="46"/>
       <c r="B22" s="38"/>
       <c r="C22" s="38"/>
       <c r="D22" s="38"/>
       <c r="E22" s="30"/>
     </row>
     <row r="23" ht="13.65" customHeight="1">
-      <c r="A23" s="37"/>
+      <c r="A23" s="46"/>
       <c r="B23" s="38"/>
       <c r="C23" s="38"/>
       <c r="D23" s="38"/>
       <c r="E23" s="30"/>
     </row>
     <row r="24" ht="13.65" customHeight="1">
-      <c r="A24" s="37"/>
+      <c r="A24" s="46"/>
       <c r="B24" s="38"/>
       <c r="C24" s="38"/>
       <c r="D24" s="38"/>
       <c r="E24" s="30"/>
     </row>
     <row r="25" ht="13.65" customHeight="1">
-      <c r="A25" s="37"/>
+      <c r="A25" s="46"/>
       <c r="B25" s="38"/>
       <c r="C25" s="38"/>
       <c r="D25" s="38"/>
       <c r="E25" s="30"/>
     </row>
     <row r="26" ht="13.65" customHeight="1">
-      <c r="A26" s="40"/>
-      <c r="B26" t="s" s="41">
-        <v>19</v>
-      </c>
-      <c r="C26" s="42"/>
-      <c r="D26" s="42"/>
+      <c r="A26" s="42"/>
+      <c r="B26" t="s" s="43">
+        <v>21</v>
+      </c>
+      <c r="C26" s="44"/>
+      <c r="D26" s="44"/>
       <c r="E26" s="30"/>
     </row>
     <row r="27" ht="57.65" customHeight="1">
       <c r="A27" t="s" s="34">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B27" s="35"/>
-      <c r="C27" s="49"/>
+      <c r="C27" s="50"/>
       <c r="D27" s="36"/>
       <c r="E27" s="30"/>
     </row>
     <row r="28" ht="13.65" customHeight="1">
-      <c r="A28" t="s" s="43">
-        <v>24</v>
+      <c r="A28" t="s" s="37">
+        <v>25</v>
       </c>
       <c r="B28" s="38"/>
-      <c r="C28" t="s" s="44">
-        <v>26</v>
+      <c r="C28" t="s" s="39">
+        <v>27</v>
       </c>
       <c r="D28" s="38"/>
       <c r="E28" s="30"/>
     </row>
     <row r="29" ht="13.65" customHeight="1">
-      <c r="A29" s="37"/>
+      <c r="A29" t="s" s="37">
+        <v>28</v>
+      </c>
       <c r="B29" s="38"/>
-      <c r="C29" s="38"/>
+      <c r="C29" t="s" s="39">
+        <v>20</v>
+      </c>
       <c r="D29" s="38"/>
       <c r="E29" s="30"/>
     </row>
     <row r="30" ht="13.65" customHeight="1">
-      <c r="A30" s="37"/>
+      <c r="A30" t="s" s="37">
+        <v>29</v>
+      </c>
       <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
+      <c r="C30" t="s" s="39">
+        <v>20</v>
+      </c>
       <c r="D30" s="38"/>
       <c r="E30" s="30"/>
     </row>
     <row r="31" ht="13.65" customHeight="1">
-      <c r="A31" s="37"/>
+      <c r="A31" s="40"/>
       <c r="B31" s="38"/>
       <c r="C31" s="38"/>
       <c r="D31" s="38"/>
       <c r="E31" s="30"/>
     </row>
     <row r="32" ht="13.65" customHeight="1">
-      <c r="A32" s="37"/>
+      <c r="A32" s="46"/>
       <c r="B32" s="38"/>
       <c r="C32" s="38"/>
       <c r="D32" s="38"/>
       <c r="E32" s="30"/>
     </row>
     <row r="33" ht="13.65" customHeight="1">
-      <c r="A33" s="40"/>
-      <c r="B33" t="s" s="41">
+      <c r="A33" s="42"/>
+      <c r="B33" t="s" s="43">
+        <v>21</v>
+      </c>
+      <c r="C33" s="44"/>
+      <c r="D33" s="44"/>
+      <c r="E33" s="30"/>
+    </row>
+    <row r="34" ht="17.1" customHeight="1">
+      <c r="A34" s="51"/>
+      <c r="B34" s="52"/>
+      <c r="C34" s="52"/>
+      <c r="D34" s="52"/>
+      <c r="E34" s="30"/>
+    </row>
+    <row r="35" ht="17.95" customHeight="1">
+      <c r="A35" t="s" s="53">
+        <v>30</v>
+      </c>
+      <c r="B35" s="54"/>
+      <c r="C35" s="54"/>
+      <c r="D35" s="54"/>
+      <c r="E35" s="30"/>
+    </row>
+    <row r="36" ht="17.95" customHeight="1">
+      <c r="A36" t="s" s="55">
+        <v>13</v>
+      </c>
+      <c r="B36" s="56"/>
+      <c r="C36" s="56"/>
+      <c r="D36" s="56"/>
+      <c r="E36" s="30"/>
+    </row>
+    <row r="37" ht="17.95" customHeight="1">
+      <c r="A37" t="s" s="57">
+        <v>31</v>
+      </c>
+      <c r="B37" s="58"/>
+      <c r="C37" s="59"/>
+      <c r="D37" s="59"/>
+      <c r="E37" s="30"/>
+    </row>
+    <row r="38" ht="57.65" customHeight="1">
+      <c r="A38" t="s" s="60">
+        <v>32</v>
+      </c>
+      <c r="B38" s="61"/>
+      <c r="C38" s="62"/>
+      <c r="D38" s="62"/>
+      <c r="E38" s="30"/>
+    </row>
+    <row r="39" ht="13.65" customHeight="1">
+      <c r="A39" t="s" s="37">
         <v>19</v>
       </c>
-      <c r="C33" s="42"/>
-      <c r="D33" s="42"/>
-      <c r="E33" s="30"/>
-    </row>
-    <row r="34" ht="17.1" customHeight="1">
-      <c r="A34" s="50"/>
-      <c r="B34" s="51"/>
-      <c r="C34" s="51"/>
-      <c r="D34" s="51"/>
-      <c r="E34" s="30"/>
-    </row>
-    <row r="35" ht="17.95" customHeight="1">
-      <c r="A35" t="s" s="52">
-        <v>27</v>
-      </c>
-      <c r="B35" s="53"/>
-      <c r="C35" s="53"/>
-      <c r="D35" s="53"/>
-      <c r="E35" s="30"/>
-    </row>
-    <row r="36" ht="17.95" customHeight="1">
-      <c r="A36" t="s" s="54">
-        <v>13</v>
-      </c>
-      <c r="B36" s="55"/>
-      <c r="C36" s="55"/>
-      <c r="D36" s="55"/>
-      <c r="E36" s="30"/>
-    </row>
-    <row r="37" ht="17.95" customHeight="1">
-      <c r="A37" t="s" s="56">
-        <v>28</v>
-      </c>
-      <c r="B37" s="57"/>
-      <c r="C37" s="58"/>
-      <c r="D37" s="58"/>
-      <c r="E37" s="30"/>
-    </row>
-    <row r="38" ht="57.65" customHeight="1">
-      <c r="A38" t="s" s="59">
-        <v>29</v>
-      </c>
-      <c r="B38" s="60"/>
-      <c r="C38" s="61"/>
-      <c r="D38" s="61"/>
-      <c r="E38" s="30"/>
-    </row>
-    <row r="39" ht="13.65" customHeight="1">
-      <c r="A39" t="s" s="43">
-        <v>30</v>
-      </c>
       <c r="B39" s="38"/>
-      <c r="C39" t="s" s="44">
-        <v>22</v>
+      <c r="C39" t="s" s="39">
+        <v>20</v>
       </c>
       <c r="D39" s="38"/>
       <c r="E39" s="30"/>
     </row>
     <row r="40" ht="13.65" customHeight="1">
-      <c r="A40" s="62"/>
+      <c r="A40" s="45"/>
       <c r="B40" s="38"/>
       <c r="C40" s="38"/>
       <c r="D40" s="38"/>
       <c r="E40" s="30"/>
     </row>
     <row r="41" ht="13.65" customHeight="1">
-      <c r="A41" s="37"/>
+      <c r="A41" s="46"/>
       <c r="B41" s="38"/>
       <c r="C41" s="38"/>
       <c r="D41" s="38"/>
       <c r="E41" s="30"/>
     </row>
     <row r="42" ht="13.65" customHeight="1">
-      <c r="A42" s="37"/>
+      <c r="A42" s="46"/>
       <c r="B42" s="38"/>
       <c r="C42" s="38"/>
       <c r="D42" s="38"/>
       <c r="E42" s="30"/>
     </row>
     <row r="43" ht="13.65" customHeight="1">
-      <c r="A43" s="37"/>
+      <c r="A43" s="46"/>
       <c r="B43" s="38"/>
       <c r="C43" s="38"/>
       <c r="D43" s="38"/>
       <c r="E43" s="30"/>
     </row>
     <row r="44" ht="13.65" customHeight="1">
-      <c r="A44" s="37"/>
-      <c r="B44" t="s" s="41">
-        <v>19</v>
-      </c>
-      <c r="C44" s="42"/>
-      <c r="D44" s="42"/>
+      <c r="A44" s="46"/>
+      <c r="B44" t="s" s="43">
+        <v>21</v>
+      </c>
+      <c r="C44" s="44"/>
+      <c r="D44" s="44"/>
       <c r="E44" s="30"/>
     </row>
     <row r="45" ht="24.65" customHeight="1">
-      <c r="A45" t="s" s="59">
-        <v>31</v>
+      <c r="A45" t="s" s="60">
+        <v>33</v>
       </c>
       <c r="B45" s="63"/>
       <c r="C45" s="64"/>
@@ -2745,52 +2763,52 @@
       <c r="E45" s="30"/>
     </row>
     <row r="46" ht="13.65" customHeight="1">
-      <c r="A46" s="37"/>
+      <c r="A46" s="46"/>
       <c r="B46" s="38"/>
       <c r="C46" s="38"/>
       <c r="D46" s="38"/>
       <c r="E46" s="30"/>
     </row>
     <row r="47" ht="13.65" customHeight="1">
-      <c r="A47" s="37"/>
+      <c r="A47" s="46"/>
       <c r="B47" s="38"/>
       <c r="C47" s="38"/>
       <c r="D47" s="38"/>
       <c r="E47" s="30"/>
     </row>
     <row r="48" ht="13.65" customHeight="1">
-      <c r="A48" s="37"/>
+      <c r="A48" s="46"/>
       <c r="B48" s="38"/>
       <c r="C48" s="38"/>
       <c r="D48" s="38"/>
       <c r="E48" s="30"/>
     </row>
     <row r="49" ht="13.65" customHeight="1">
-      <c r="A49" s="37"/>
+      <c r="A49" s="46"/>
       <c r="B49" s="38"/>
       <c r="C49" s="38"/>
       <c r="D49" s="38"/>
       <c r="E49" s="30"/>
     </row>
     <row r="50" ht="13.65" customHeight="1">
-      <c r="A50" s="37"/>
+      <c r="A50" s="46"/>
       <c r="B50" s="38"/>
       <c r="C50" s="38"/>
       <c r="D50" s="38"/>
       <c r="E50" s="30"/>
     </row>
     <row r="51" ht="13.65" customHeight="1">
-      <c r="A51" s="37"/>
-      <c r="B51" t="s" s="41">
-        <v>19</v>
-      </c>
-      <c r="C51" s="42"/>
-      <c r="D51" s="42"/>
+      <c r="A51" s="46"/>
+      <c r="B51" t="s" s="43">
+        <v>21</v>
+      </c>
+      <c r="C51" s="44"/>
+      <c r="D51" s="44"/>
       <c r="E51" s="30"/>
     </row>
     <row r="52" ht="46.65" customHeight="1">
-      <c r="A52" t="s" s="59">
-        <v>32</v>
+      <c r="A52" t="s" s="60">
+        <v>34</v>
       </c>
       <c r="B52" s="64"/>
       <c r="C52" s="64"/>
@@ -2798,52 +2816,52 @@
       <c r="E52" s="30"/>
     </row>
     <row r="53" ht="13.65" customHeight="1">
-      <c r="A53" s="37"/>
+      <c r="A53" s="46"/>
       <c r="B53" s="38"/>
       <c r="C53" s="38"/>
       <c r="D53" s="38"/>
       <c r="E53" s="30"/>
     </row>
     <row r="54" ht="13.65" customHeight="1">
-      <c r="A54" s="37"/>
+      <c r="A54" s="46"/>
       <c r="B54" s="38"/>
       <c r="C54" s="38"/>
       <c r="D54" s="38"/>
       <c r="E54" s="30"/>
     </row>
     <row r="55" ht="13.65" customHeight="1">
-      <c r="A55" s="37"/>
+      <c r="A55" s="46"/>
       <c r="B55" s="38"/>
       <c r="C55" s="38"/>
       <c r="D55" s="38"/>
       <c r="E55" s="30"/>
     </row>
     <row r="56" ht="13.65" customHeight="1">
-      <c r="A56" s="37"/>
+      <c r="A56" s="46"/>
       <c r="B56" s="38"/>
       <c r="C56" s="38"/>
       <c r="D56" s="38"/>
       <c r="E56" s="30"/>
     </row>
     <row r="57" ht="13.65" customHeight="1">
-      <c r="A57" s="37"/>
+      <c r="A57" s="46"/>
       <c r="B57" s="38"/>
       <c r="C57" s="38"/>
       <c r="D57" s="38"/>
       <c r="E57" s="30"/>
     </row>
     <row r="58" ht="13.65" customHeight="1">
-      <c r="A58" s="37"/>
-      <c r="B58" t="s" s="41">
-        <v>19</v>
-      </c>
-      <c r="C58" s="42"/>
-      <c r="D58" s="42"/>
+      <c r="A58" s="46"/>
+      <c r="B58" t="s" s="43">
+        <v>21</v>
+      </c>
+      <c r="C58" s="44"/>
+      <c r="D58" s="44"/>
       <c r="E58" s="30"/>
     </row>
     <row r="59" ht="35.65" customHeight="1">
-      <c r="A59" t="s" s="59">
-        <v>33</v>
+      <c r="A59" t="s" s="60">
+        <v>35</v>
       </c>
       <c r="B59" s="64"/>
       <c r="C59" s="64"/>
@@ -2851,52 +2869,52 @@
       <c r="E59" s="30"/>
     </row>
     <row r="60" ht="13.65" customHeight="1">
-      <c r="A60" s="37"/>
+      <c r="A60" s="46"/>
       <c r="B60" s="38"/>
       <c r="C60" s="38"/>
       <c r="D60" s="38"/>
       <c r="E60" s="30"/>
     </row>
     <row r="61" ht="13.65" customHeight="1">
-      <c r="A61" s="37"/>
+      <c r="A61" s="46"/>
       <c r="B61" s="38"/>
       <c r="C61" s="38"/>
       <c r="D61" s="38"/>
       <c r="E61" s="30"/>
     </row>
     <row r="62" ht="13.65" customHeight="1">
-      <c r="A62" s="37"/>
+      <c r="A62" s="46"/>
       <c r="B62" s="38"/>
       <c r="C62" s="38"/>
       <c r="D62" s="38"/>
       <c r="E62" s="30"/>
     </row>
     <row r="63" ht="13.65" customHeight="1">
-      <c r="A63" s="37"/>
+      <c r="A63" s="46"/>
       <c r="B63" s="38"/>
       <c r="C63" s="38"/>
       <c r="D63" s="38"/>
       <c r="E63" s="30"/>
     </row>
     <row r="64" ht="13.65" customHeight="1">
-      <c r="A64" s="37"/>
+      <c r="A64" s="46"/>
       <c r="B64" s="38"/>
       <c r="C64" s="38"/>
       <c r="D64" s="38"/>
       <c r="E64" s="30"/>
     </row>
     <row r="65" ht="13.65" customHeight="1">
-      <c r="A65" s="37"/>
-      <c r="B65" t="s" s="41">
-        <v>19</v>
-      </c>
-      <c r="C65" s="42"/>
-      <c r="D65" s="42"/>
+      <c r="A65" s="46"/>
+      <c r="B65" t="s" s="43">
+        <v>21</v>
+      </c>
+      <c r="C65" s="44"/>
+      <c r="D65" s="44"/>
       <c r="E65" s="30"/>
     </row>
     <row r="66" ht="46.65" customHeight="1">
-      <c r="A66" t="s" s="59">
-        <v>34</v>
+      <c r="A66" t="s" s="60">
+        <v>36</v>
       </c>
       <c r="B66" s="64"/>
       <c r="C66" s="64"/>
@@ -2904,52 +2922,52 @@
       <c r="E66" s="30"/>
     </row>
     <row r="67" ht="13.65" customHeight="1">
-      <c r="A67" s="37"/>
+      <c r="A67" s="46"/>
       <c r="B67" s="38"/>
       <c r="C67" s="38"/>
       <c r="D67" s="38"/>
       <c r="E67" s="30"/>
     </row>
     <row r="68" ht="13.65" customHeight="1">
-      <c r="A68" s="37"/>
+      <c r="A68" s="46"/>
       <c r="B68" s="38"/>
       <c r="C68" s="38"/>
       <c r="D68" s="38"/>
       <c r="E68" s="30"/>
     </row>
     <row r="69" ht="13.65" customHeight="1">
-      <c r="A69" s="37"/>
+      <c r="A69" s="46"/>
       <c r="B69" s="38"/>
       <c r="C69" s="38"/>
       <c r="D69" s="38"/>
       <c r="E69" s="30"/>
     </row>
     <row r="70" ht="13.65" customHeight="1">
-      <c r="A70" s="37"/>
+      <c r="A70" s="46"/>
       <c r="B70" s="38"/>
       <c r="C70" s="38"/>
       <c r="D70" s="38"/>
       <c r="E70" s="30"/>
     </row>
     <row r="71" ht="13.65" customHeight="1">
-      <c r="A71" s="37"/>
+      <c r="A71" s="46"/>
       <c r="B71" s="38"/>
       <c r="C71" s="38"/>
       <c r="D71" s="38"/>
       <c r="E71" s="30"/>
     </row>
     <row r="72" ht="13.65" customHeight="1">
-      <c r="A72" s="37"/>
-      <c r="B72" t="s" s="41">
-        <v>19</v>
-      </c>
-      <c r="C72" s="42"/>
-      <c r="D72" s="42"/>
+      <c r="A72" s="46"/>
+      <c r="B72" t="s" s="43">
+        <v>21</v>
+      </c>
+      <c r="C72" s="44"/>
+      <c r="D72" s="44"/>
       <c r="E72" s="30"/>
     </row>
     <row r="73" ht="46.65" customHeight="1">
-      <c r="A73" t="s" s="59">
-        <v>35</v>
+      <c r="A73" t="s" s="60">
+        <v>37</v>
       </c>
       <c r="B73" s="64"/>
       <c r="C73" s="64"/>
@@ -2957,52 +2975,52 @@
       <c r="E73" s="30"/>
     </row>
     <row r="74" ht="13.65" customHeight="1">
-      <c r="A74" s="37"/>
+      <c r="A74" s="46"/>
       <c r="B74" s="38"/>
       <c r="C74" s="38"/>
       <c r="D74" s="38"/>
       <c r="E74" s="30"/>
     </row>
     <row r="75" ht="13.65" customHeight="1">
-      <c r="A75" s="37"/>
+      <c r="A75" s="46"/>
       <c r="B75" s="38"/>
       <c r="C75" s="38"/>
       <c r="D75" s="38"/>
       <c r="E75" s="30"/>
     </row>
     <row r="76" ht="13.65" customHeight="1">
-      <c r="A76" s="37"/>
+      <c r="A76" s="46"/>
       <c r="B76" s="38"/>
       <c r="C76" s="38"/>
       <c r="D76" s="38"/>
       <c r="E76" s="30"/>
     </row>
     <row r="77" ht="13.65" customHeight="1">
-      <c r="A77" s="37"/>
+      <c r="A77" s="46"/>
       <c r="B77" s="38"/>
       <c r="C77" s="38"/>
       <c r="D77" s="38"/>
       <c r="E77" s="30"/>
     </row>
     <row r="78" ht="13.65" customHeight="1">
-      <c r="A78" s="37"/>
+      <c r="A78" s="46"/>
       <c r="B78" s="38"/>
       <c r="C78" s="38"/>
       <c r="D78" s="38"/>
       <c r="E78" s="30"/>
     </row>
     <row r="79" ht="13.65" customHeight="1">
-      <c r="A79" s="37"/>
-      <c r="B79" t="s" s="41">
-        <v>19</v>
-      </c>
-      <c r="C79" s="42"/>
-      <c r="D79" s="42"/>
+      <c r="A79" s="46"/>
+      <c r="B79" t="s" s="43">
+        <v>21</v>
+      </c>
+      <c r="C79" s="44"/>
+      <c r="D79" s="44"/>
       <c r="E79" s="30"/>
     </row>
     <row r="80" ht="35.65" customHeight="1">
-      <c r="A80" t="s" s="59">
-        <v>36</v>
+      <c r="A80" t="s" s="60">
+        <v>38</v>
       </c>
       <c r="B80" s="64"/>
       <c r="C80" s="64"/>
@@ -3010,52 +3028,54 @@
       <c r="E80" s="30"/>
     </row>
     <row r="81" ht="13.65" customHeight="1">
-      <c r="A81" s="37"/>
+      <c r="A81" s="46"/>
       <c r="B81" s="38"/>
       <c r="C81" s="38"/>
       <c r="D81" s="38"/>
       <c r="E81" s="30"/>
     </row>
     <row r="82" ht="13.65" customHeight="1">
-      <c r="A82" s="37"/>
+      <c r="A82" s="46"/>
       <c r="B82" s="38"/>
       <c r="C82" s="38"/>
       <c r="D82" s="38"/>
       <c r="E82" s="30"/>
     </row>
     <row r="83" ht="13.65" customHeight="1">
-      <c r="A83" s="37"/>
+      <c r="A83" s="46"/>
       <c r="B83" s="38"/>
       <c r="C83" s="38"/>
       <c r="D83" s="38"/>
       <c r="E83" s="30"/>
     </row>
     <row r="84" ht="13.65" customHeight="1">
-      <c r="A84" s="37"/>
+      <c r="A84" s="46"/>
       <c r="B84" s="38"/>
       <c r="C84" s="38"/>
       <c r="D84" s="38"/>
       <c r="E84" s="30"/>
     </row>
     <row r="85" ht="13.65" customHeight="1">
-      <c r="A85" s="37"/>
+      <c r="A85" s="46"/>
       <c r="B85" s="38"/>
       <c r="C85" s="38"/>
       <c r="D85" s="38"/>
       <c r="E85" s="30"/>
     </row>
     <row r="86" ht="13.65" customHeight="1">
-      <c r="A86" s="37"/>
-      <c r="B86" t="s" s="41">
-        <v>19</v>
-      </c>
-      <c r="C86" s="42"/>
-      <c r="D86" s="42"/>
+      <c r="A86" s="46"/>
+      <c r="B86" t="s" s="43">
+        <v>21</v>
+      </c>
+      <c r="C86" s="44"/>
+      <c r="D86" s="44"/>
       <c r="E86" s="65"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C39" r:id="rId1" location="" tooltip="" display=""/>
+    <hyperlink ref="C6" r:id="rId1" location="" tooltip="" display=""/>
+    <hyperlink ref="C29" r:id="rId2" location="" tooltip="" display=""/>
+    <hyperlink ref="C30" r:id="rId3" location="" tooltip="" display=""/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.492126" footer="0.492126"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="landscape" pageOrder="downThenOver"/>

</xml_diff>